<commit_message>
Split 'retrieves' layer into concepts, demographics, retrieves; use common helper libraries
</commit_message>
<xml_diff>
--- a/src/main/resources/opencpg/covid19/ed/owl/Data Elements.xlsx
+++ b/src/main/resources/opencpg/covid19/ed/owl/Data Elements.xlsx
@@ -317,9 +317,6 @@
     <t>SCTID: 40617009  | Artificial respiration (procedure)</t>
   </si>
   <si>
-    <t xml:space="preserve">Dobutamine </t>
-  </si>
-  <si>
     <t>Medication</t>
   </si>
   <si>
@@ -699,6 +696,9 @@
   </si>
   <si>
     <t>4h</t>
+  </si>
+  <si>
+    <t>Dobutamine</t>
   </si>
 </sst>
 </file>
@@ -1190,7 +1190,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F26" sqref="F26"/>
+      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1217,19 +1217,19 @@
         <v>1</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I1" s="7" t="s">
         <v>3</v>
@@ -1414,14 +1414,14 @@
         <v>12</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F7" s="14" t="s">
         <v>28</v>
       </c>
       <c r="G7" s="51"/>
       <c r="H7" s="53" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I7" s="15"/>
       <c r="J7" s="19">
@@ -1441,7 +1441,7 @@
         <v>29</v>
       </c>
       <c r="C8" s="53" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D8" s="17" t="s">
         <v>12</v>
@@ -1837,17 +1837,17 @@
     <row r="21" spans="1:17" ht="14.25">
       <c r="A21" s="9"/>
       <c r="B21" s="20" t="s">
+        <v>196</v>
+      </c>
+      <c r="C21" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="C21" s="16" t="s">
+      <c r="D21" s="17" t="s">
         <v>70</v>
-      </c>
-      <c r="D21" s="17" t="s">
-        <v>71</v>
       </c>
       <c r="E21" s="18"/>
       <c r="F21" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G21" s="51"/>
       <c r="H21" s="9"/>
@@ -1860,7 +1860,7 @@
       <c r="M21" s="9"/>
       <c r="N21" s="9"/>
       <c r="O21" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="P21" s="21">
         <v>3616</v>
@@ -1870,17 +1870,17 @@
     <row r="22" spans="1:17" ht="14.25">
       <c r="A22" s="9"/>
       <c r="B22" s="20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C22" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="D22" s="17" t="s">
         <v>70</v>
-      </c>
-      <c r="D22" s="17" t="s">
-        <v>71</v>
       </c>
       <c r="E22" s="18"/>
       <c r="F22" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G22" s="51"/>
       <c r="H22" s="9"/>
@@ -1893,7 +1893,7 @@
       <c r="M22" s="9"/>
       <c r="N22" s="9"/>
       <c r="O22" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="P22" s="29">
         <v>3992</v>
@@ -1903,17 +1903,17 @@
     <row r="23" spans="1:17" ht="14.25">
       <c r="A23" s="9"/>
       <c r="B23" s="20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C23" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="D23" s="17" t="s">
         <v>70</v>
-      </c>
-      <c r="D23" s="17" t="s">
-        <v>71</v>
       </c>
       <c r="E23" s="18"/>
       <c r="F23" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G23" s="51"/>
       <c r="H23" s="9"/>
@@ -1934,17 +1934,17 @@
     <row r="24" spans="1:17" ht="14.25">
       <c r="A24" s="9"/>
       <c r="B24" s="20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C24" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="D24" s="17" t="s">
         <v>70</v>
-      </c>
-      <c r="D24" s="17" t="s">
-        <v>71</v>
       </c>
       <c r="E24" s="18"/>
       <c r="F24" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G24" s="51"/>
       <c r="H24" s="9"/>
@@ -1965,17 +1965,17 @@
     <row r="25" spans="1:17" ht="14.25">
       <c r="A25" s="9"/>
       <c r="B25" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C25" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="D25" s="17" t="s">
         <v>70</v>
-      </c>
-      <c r="D25" s="17" t="s">
-        <v>71</v>
       </c>
       <c r="E25" s="18"/>
       <c r="F25" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G25" s="51"/>
       <c r="H25" s="9"/>
@@ -1988,7 +1988,7 @@
       <c r="M25" s="9"/>
       <c r="N25" s="9"/>
       <c r="O25" s="16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="P25" s="29">
         <v>3628</v>
@@ -1998,17 +1998,17 @@
     <row r="26" spans="1:17" ht="12.75">
       <c r="A26" s="9"/>
       <c r="B26" s="22" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D26" s="17" t="s">
         <v>12</v>
       </c>
       <c r="E26" s="10"/>
       <c r="F26" s="14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G26" s="50"/>
       <c r="H26" s="9"/>
@@ -2019,7 +2019,7 @@
       <c r="M26" s="9"/>
       <c r="N26" s="9"/>
       <c r="O26" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="P26" s="9"/>
       <c r="Q26" s="34"/>
@@ -2027,17 +2027,17 @@
     <row r="27" spans="1:17" ht="12.75">
       <c r="A27" s="9"/>
       <c r="B27" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C27" s="51" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D27" s="17" t="s">
         <v>12</v>
       </c>
       <c r="E27" s="10"/>
       <c r="F27" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G27" s="51"/>
       <c r="H27" s="9"/>
@@ -2047,7 +2047,7 @@
       </c>
       <c r="K27" s="9"/>
       <c r="L27" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="M27" s="9"/>
       <c r="N27" s="28">
@@ -2060,17 +2060,17 @@
     <row r="28" spans="1:17" ht="12.75">
       <c r="A28" s="9"/>
       <c r="B28" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C28" s="51" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D28" s="17" t="s">
         <v>12</v>
       </c>
       <c r="E28" s="10"/>
       <c r="F28" s="14" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G28" s="51"/>
       <c r="H28" s="9"/>
@@ -2080,7 +2080,7 @@
       </c>
       <c r="K28" s="9"/>
       <c r="L28" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="M28" s="9"/>
       <c r="N28" s="28">
@@ -2093,10 +2093,10 @@
     <row r="29" spans="1:17" ht="12.75">
       <c r="A29" s="9"/>
       <c r="B29" s="22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C29" s="51" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D29" s="17" t="s">
         <v>12</v>
@@ -2111,7 +2111,7 @@
       </c>
       <c r="K29" s="9"/>
       <c r="L29" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="M29" s="9"/>
       <c r="N29" s="28">
@@ -2124,17 +2124,17 @@
     <row r="30" spans="1:17" ht="14.25">
       <c r="A30" s="9"/>
       <c r="B30" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C30" s="51" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D30" s="17" t="s">
         <v>12</v>
       </c>
       <c r="E30" s="10"/>
       <c r="F30" s="14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G30" s="51"/>
       <c r="H30" s="9"/>
@@ -2144,7 +2144,7 @@
       </c>
       <c r="K30" s="9"/>
       <c r="L30" s="16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M30" s="9"/>
       <c r="N30" s="28">
@@ -2157,17 +2157,17 @@
     <row r="31" spans="1:17" ht="12.75">
       <c r="A31" s="9"/>
       <c r="B31" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C31" s="51" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D31" s="17" t="s">
         <v>12</v>
       </c>
       <c r="E31" s="10"/>
       <c r="F31" s="14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G31" s="51"/>
       <c r="H31" s="9"/>
@@ -2177,7 +2177,7 @@
       </c>
       <c r="K31" s="9"/>
       <c r="L31" s="9" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="M31" s="9"/>
       <c r="N31" s="28">
@@ -2190,17 +2190,17 @@
     <row r="32" spans="1:17" ht="14.25">
       <c r="A32" s="9"/>
       <c r="B32" s="20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C32" s="51" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D32" s="17" t="s">
         <v>12</v>
       </c>
       <c r="E32" s="10"/>
       <c r="F32" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G32" s="51"/>
       <c r="H32" s="31"/>
@@ -2210,7 +2210,7 @@
       </c>
       <c r="K32" s="9"/>
       <c r="L32" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M32" s="9"/>
       <c r="N32" s="32">
@@ -2223,17 +2223,17 @@
     <row r="33" spans="1:17" ht="14.25">
       <c r="A33" s="9"/>
       <c r="B33" s="20" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C33" s="51" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D33" s="17" t="s">
         <v>12</v>
       </c>
       <c r="E33" s="10"/>
       <c r="F33" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G33" s="51"/>
       <c r="H33" s="9"/>
@@ -2243,11 +2243,11 @@
       </c>
       <c r="K33" s="9"/>
       <c r="L33" s="16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="M33" s="9"/>
       <c r="N33" s="32" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O33" s="9"/>
       <c r="P33" s="9"/>
@@ -2256,17 +2256,17 @@
     <row r="34" spans="1:17" ht="12.75">
       <c r="A34" s="9"/>
       <c r="B34" s="16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C34" s="51" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D34" s="17" t="s">
         <v>12</v>
       </c>
       <c r="E34" s="10"/>
       <c r="F34" s="14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G34" s="51"/>
       <c r="H34" s="9"/>
@@ -2276,7 +2276,7 @@
       </c>
       <c r="K34" s="9"/>
       <c r="L34" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M34" s="9"/>
       <c r="N34" s="28">
@@ -2289,17 +2289,17 @@
     <row r="35" spans="1:17" ht="12.75">
       <c r="A35" s="9"/>
       <c r="B35" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C35" s="51" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D35" s="17" t="s">
         <v>12</v>
       </c>
       <c r="E35" s="10"/>
       <c r="F35" s="14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G35" s="51"/>
       <c r="H35" s="9"/>
@@ -2309,7 +2309,7 @@
       </c>
       <c r="K35" s="9"/>
       <c r="L35" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="M35" s="9"/>
       <c r="N35" s="28">
@@ -2322,17 +2322,17 @@
     <row r="36" spans="1:17" ht="14.25">
       <c r="A36" s="9"/>
       <c r="B36" s="20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C36" s="51" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D36" s="17" t="s">
         <v>12</v>
       </c>
       <c r="E36" s="10"/>
       <c r="F36" s="14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G36" s="51"/>
       <c r="H36" s="9"/>
@@ -2342,14 +2342,14 @@
       </c>
       <c r="K36" s="9"/>
       <c r="L36" s="16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="M36" s="9"/>
       <c r="N36" s="33">
         <v>85049</v>
       </c>
       <c r="O36" s="16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="P36" s="9"/>
       <c r="Q36" s="34"/>
@@ -2357,17 +2357,17 @@
     <row r="37" spans="1:17" ht="18.75" customHeight="1">
       <c r="A37" s="9"/>
       <c r="B37" s="34" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C37" s="51" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D37" s="17" t="s">
         <v>12</v>
       </c>
       <c r="E37" s="10"/>
       <c r="F37" s="14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H37" s="9"/>
       <c r="I37" s="15"/>
@@ -2376,7 +2376,7 @@
       </c>
       <c r="K37" s="9"/>
       <c r="L37" s="16" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M37" s="9"/>
       <c r="N37" s="33">
@@ -2389,17 +2389,17 @@
     <row r="38" spans="1:17" ht="14.25">
       <c r="A38" s="9"/>
       <c r="B38" s="34" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C38" s="51" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D38" s="17" t="s">
         <v>12</v>
       </c>
       <c r="E38" s="10"/>
       <c r="F38" s="14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H38" s="9"/>
       <c r="I38" s="15"/>
@@ -2408,7 +2408,7 @@
       </c>
       <c r="K38" s="9"/>
       <c r="L38" s="29" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="M38" s="9"/>
       <c r="N38" s="33">
@@ -2421,30 +2421,30 @@
     <row r="39" spans="1:17" ht="12.75">
       <c r="A39" s="9"/>
       <c r="B39" s="42" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C39" s="26" t="s">
         <v>24</v>
       </c>
       <c r="D39" s="43" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E39" s="40"/>
       <c r="F39" s="44" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G39" s="42" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H39" s="9"/>
       <c r="I39" s="45" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J39" s="41">
         <v>165612</v>
       </c>
       <c r="K39" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L39" s="9"/>
       <c r="M39" s="9"/>
@@ -2456,30 +2456,30 @@
     <row r="40" spans="1:17" ht="12.75">
       <c r="A40" s="9"/>
       <c r="B40" s="42" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C40" s="26" t="s">
         <v>24</v>
       </c>
       <c r="D40" s="43" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E40" s="40"/>
       <c r="F40" s="46" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G40" s="52" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H40" s="9"/>
       <c r="I40" s="45" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J40" s="41">
         <v>165623</v>
       </c>
       <c r="K40" s="24" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L40" s="9"/>
       <c r="M40" s="9"/>
@@ -2491,28 +2491,28 @@
     <row r="41" spans="1:17" ht="12.75">
       <c r="A41" s="9"/>
       <c r="B41" s="22" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C41" s="26" t="s">
         <v>24</v>
       </c>
       <c r="D41" s="43" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E41" s="10"/>
       <c r="F41" s="14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G41" s="50"/>
       <c r="H41" s="9"/>
       <c r="I41" s="15" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J41" s="41">
         <v>142474</v>
       </c>
       <c r="K41" s="24" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L41" s="9"/>
       <c r="M41" s="9"/>
@@ -2524,28 +2524,28 @@
     <row r="42" spans="1:17" ht="12.75">
       <c r="A42" s="9"/>
       <c r="B42" s="9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C42" s="26" t="s">
         <v>24</v>
       </c>
       <c r="D42" s="43" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E42" s="10"/>
       <c r="F42" s="14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G42" s="51"/>
       <c r="H42" s="9"/>
       <c r="I42" s="15" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J42" s="41">
         <v>142473</v>
       </c>
       <c r="K42" s="24" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L42" s="9"/>
       <c r="M42" s="9"/>
@@ -2557,28 +2557,28 @@
     <row r="43" spans="1:17" ht="12.75">
       <c r="A43" s="9"/>
       <c r="B43" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C43" s="26" t="s">
         <v>24</v>
       </c>
       <c r="D43" s="43" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E43" s="10"/>
       <c r="F43" s="14" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G43" s="51"/>
       <c r="H43" s="9"/>
       <c r="I43" s="15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J43" s="41">
         <v>139069</v>
       </c>
       <c r="K43" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L43" s="9"/>
       <c r="M43" s="9"/>
@@ -2590,28 +2590,28 @@
     <row r="44" spans="1:17" ht="12.75">
       <c r="A44" s="9"/>
       <c r="B44" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C44" s="26" t="s">
         <v>24</v>
       </c>
       <c r="D44" s="43" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E44" s="10"/>
       <c r="F44" s="14" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G44" s="51"/>
       <c r="H44" s="9"/>
       <c r="I44" s="15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J44" s="41">
         <v>903</v>
       </c>
       <c r="K44" s="24" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="L44" s="9"/>
       <c r="M44" s="9"/>
@@ -2623,17 +2623,17 @@
     <row r="45" spans="1:17" ht="12.75">
       <c r="A45" s="9"/>
       <c r="B45" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C45" s="26" t="s">
         <v>24</v>
       </c>
       <c r="D45" s="43" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E45" s="10"/>
       <c r="F45" s="14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G45" s="51"/>
       <c r="H45" s="9"/>
@@ -2642,7 +2642,7 @@
         <v>1295</v>
       </c>
       <c r="K45" s="24" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L45" s="9"/>
       <c r="M45" s="9"/>
@@ -2654,28 +2654,28 @@
     <row r="46" spans="1:17" ht="14.25">
       <c r="A46" s="9"/>
       <c r="B46" s="16" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C46" s="26" t="s">
         <v>24</v>
       </c>
       <c r="D46" s="43" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E46" s="10"/>
       <c r="F46" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G46" s="51"/>
       <c r="H46" s="9"/>
       <c r="I46" s="15" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J46" s="21">
         <v>119270</v>
       </c>
       <c r="K46" s="47" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L46" s="9"/>
       <c r="M46" s="9"/>
@@ -2687,28 +2687,28 @@
     <row r="47" spans="1:17" ht="12.75">
       <c r="A47" s="9"/>
       <c r="B47" s="16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C47" s="9" t="s">
         <v>24</v>
       </c>
       <c r="D47" s="43" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E47" s="10"/>
       <c r="F47" s="14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G47" s="51"/>
       <c r="H47" s="9"/>
       <c r="I47" s="15" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J47" s="41">
         <v>145830</v>
       </c>
       <c r="K47" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L47" s="9"/>
       <c r="M47" s="9"/>
@@ -2720,28 +2720,28 @@
     <row r="48" spans="1:17" s="34" customFormat="1" ht="12.75">
       <c r="A48" s="51"/>
       <c r="B48" s="51" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C48" s="42" t="s">
         <v>24</v>
       </c>
       <c r="D48" s="43" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E48" s="18"/>
       <c r="F48" s="14" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G48" s="51"/>
       <c r="H48" s="51"/>
       <c r="I48" s="15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J48" s="19">
         <v>115115</v>
       </c>
       <c r="K48" s="24" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="L48" s="51"/>
       <c r="M48" s="51"/>
@@ -2752,7 +2752,7 @@
     <row r="49" spans="1:17" ht="12.75">
       <c r="A49" s="9"/>
       <c r="B49" s="9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C49" s="26" t="s">
         <v>15</v>
@@ -2762,7 +2762,7 @@
       </c>
       <c r="E49" s="10"/>
       <c r="F49" s="14" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G49" s="51"/>
       <c r="H49" s="9"/>
@@ -2781,7 +2781,7 @@
     <row r="50" spans="1:17" ht="12.75">
       <c r="A50" s="9"/>
       <c r="B50" s="48" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C50" s="9" t="s">
         <v>15</v>
@@ -2791,7 +2791,7 @@
       </c>
       <c r="E50" s="10"/>
       <c r="F50" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G50" s="48"/>
       <c r="H50" s="9"/>
@@ -2801,7 +2801,7 @@
       </c>
       <c r="K50" s="9"/>
       <c r="L50" s="9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M50" s="9"/>
       <c r="N50" s="9"/>
@@ -2812,28 +2812,28 @@
     <row r="51" spans="1:17" ht="12.75">
       <c r="A51" s="9"/>
       <c r="B51" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C51" s="26" t="s">
         <v>24</v>
       </c>
       <c r="D51" s="43" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E51" s="10"/>
       <c r="F51" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G51" s="51"/>
       <c r="H51" s="9"/>
       <c r="I51" s="15" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J51" s="19">
         <v>116505</v>
       </c>
       <c r="K51" s="9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L51" s="9"/>
       <c r="M51" s="9"/>
@@ -2845,7 +2845,7 @@
     <row r="52" spans="1:17" ht="12.75">
       <c r="A52" s="9"/>
       <c r="B52" s="48" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C52" s="42" t="s">
         <v>15</v>
@@ -2855,7 +2855,7 @@
       </c>
       <c r="E52" s="10"/>
       <c r="F52" s="14" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G52" s="48"/>
       <c r="H52" s="9"/>
@@ -2864,7 +2864,7 @@
         <v>135703</v>
       </c>
       <c r="K52" s="9" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L52" s="9"/>
       <c r="M52" s="9"/>
@@ -2876,28 +2876,28 @@
     <row r="53" spans="1:17" ht="14.25">
       <c r="A53" s="9"/>
       <c r="B53" s="20" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C53" s="16" t="s">
         <v>24</v>
       </c>
       <c r="D53" s="43" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E53" s="18"/>
       <c r="F53" s="14" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G53" s="51"/>
       <c r="H53" s="9"/>
       <c r="I53" s="15" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J53" s="21">
         <v>116031</v>
       </c>
       <c r="K53" s="29" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="L53" s="9"/>
       <c r="M53" s="9"/>
@@ -2909,13 +2909,13 @@
     <row r="54" spans="1:17" ht="18" customHeight="1">
       <c r="A54" s="9"/>
       <c r="B54" s="20" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C54" s="16" t="s">
         <v>15</v>
       </c>
       <c r="D54" s="17" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E54" s="10"/>
       <c r="F54" s="11"/>
@@ -2936,24 +2936,24 @@
     <row r="55" spans="1:17" ht="18" customHeight="1">
       <c r="A55" s="9"/>
       <c r="B55" s="20" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C55" s="16" t="s">
         <v>24</v>
       </c>
       <c r="D55" s="17" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E55" s="10"/>
       <c r="F55" s="14" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G55" s="51"/>
       <c r="H55" s="9"/>
       <c r="I55" s="12"/>
       <c r="J55" s="13"/>
       <c r="K55" s="29" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L55" s="9"/>
       <c r="M55" s="9"/>
@@ -2965,26 +2965,26 @@
     <row r="56" spans="1:17" ht="12.75">
       <c r="A56" s="9"/>
       <c r="B56" s="20" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C56" s="16" t="s">
         <v>24</v>
       </c>
       <c r="D56" s="17" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E56" s="10"/>
       <c r="F56" s="14" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G56" s="51"/>
       <c r="H56" s="9"/>
       <c r="I56" s="12"/>
       <c r="J56" s="49" t="s">
+        <v>172</v>
+      </c>
+      <c r="K56" s="29" t="s">
         <v>173</v>
-      </c>
-      <c r="K56" s="29" t="s">
-        <v>174</v>
       </c>
       <c r="L56" s="9"/>
       <c r="M56" s="9"/>
@@ -2996,26 +2996,26 @@
     <row r="57" spans="1:17" ht="12.75">
       <c r="A57" s="9"/>
       <c r="B57" s="20" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C57" s="16" t="s">
         <v>24</v>
       </c>
       <c r="D57" s="17" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E57" s="10"/>
       <c r="F57" s="14" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G57" s="51"/>
       <c r="H57" s="9"/>
       <c r="I57" s="12"/>
       <c r="J57" s="49" t="s">
+        <v>172</v>
+      </c>
+      <c r="K57" s="29" t="s">
         <v>173</v>
-      </c>
-      <c r="K57" s="29" t="s">
-        <v>174</v>
       </c>
       <c r="L57" s="9"/>
       <c r="M57" s="9"/>

</xml_diff>